<commit_message>
Scrum Master Files Updated
Update files:
Scrum Board for sprint 2.
Burndown Chart for sprint2.
</commit_message>
<xml_diff>
--- a/Project_Management/Sprint2/Burndown chart.xlsx
+++ b/Project_Management/Sprint2/Burndown chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbern\OneDrive\Documentos\GitHub\SE2324_55204_56837_58119_58427_58535_59472\Project_Management\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D275901-F913-4505-8151-C4F4669980FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8808B7-04B8-4BCC-8760-A514AE75B6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>Perceber funcionalidades do FreeCol</t>
-  </si>
-  <si>
-    <t>0.5</t>
   </si>
 </sst>
 </file>
@@ -837,16 +834,16 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -954,16 +951,16 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2222,7 +2219,7 @@
   <dimension ref="B1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2367,11 +2364,13 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
-      <c r="I6" s="10" t="s">
-        <v>20</v>
+      <c r="I6" s="10">
+        <v>0.5</v>
       </c>
       <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="K6" s="10">
+        <v>0.5</v>
+      </c>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
@@ -2394,16 +2393,18 @@
       <c r="E7" s="13"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="14"/>
+      <c r="H7" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="I7" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="14">
+        <v>0.5</v>
+      </c>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
@@ -2725,19 +2726,19 @@
       </c>
       <c r="H20" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I20" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K20" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
@@ -2772,19 +2773,19 @@
       </c>
       <c r="H21" s="22">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="I21" s="22">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="J21" s="20">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K21" s="20">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>

</xml_diff>